<commit_message>
Fix multiple placeholders in one cell
</commit_message>
<xml_diff>
--- a/tests/Resources/rich_payment_template.xlsx
+++ b/tests/Resources/rich_payment_template.xlsx
@@ -20,18 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">Заголовок</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Контент</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Дата</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Автор</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complex Content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author</t>
   </si>
   <si>
     <t xml:space="preserve">{title}</t>
@@ -58,6 +61,37 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Next line</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">From {author} in {date}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{foo}, {foo} and {bar}</t>
     </r>
   </si>
   <si>
@@ -80,7 +114,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -117,13 +151,25 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB3CAC7"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -160,7 +206,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,6 +217,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -198,7 +252,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB3CAC7"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -253,10 +307,13 @@
   <dimension ref="A2:J4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.9"/>
+  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -265,34 +322,41 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>2</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="4"/>
       <c r="H4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>